<commit_message>
working hours was updated.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AF37E05-5201-4177-ADA8-B91F6EC00765}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76CF26FE-B994-4995-95B4-31913D91BD97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="5">
   <si>
     <t>Developer1</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>1.5</t>
+  </si>
+  <si>
+    <t>2.5</t>
   </si>
 </sst>
 </file>
@@ -367,16 +370,16 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -387,7 +390,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44272</v>
       </c>
@@ -398,7 +401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44275</v>
       </c>
@@ -409,7 +412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44283</v>
       </c>
@@ -420,7 +423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44284</v>
       </c>
@@ -431,99 +434,104 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>44286</v>
+      </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>

</xml_diff>

<commit_message>
refactor on db design. createDatabase utilty was added to the solution.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\personal\Erko_Project\ErkoSMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C68E343-0816-4DE2-9BE9-734B4C352F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F38FA6-B409-454A-8A19-6162FC68321C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3315" yWindow="3315" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
   <si>
     <t>Developer1</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>3</t>
   </si>
 </sst>
 </file>
@@ -373,16 +382,16 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -393,7 +402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44272</v>
       </c>
@@ -404,7 +413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44275</v>
       </c>
@@ -415,7 +424,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44283</v>
       </c>
@@ -426,7 +435,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44284</v>
       </c>
@@ -437,16 +446,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44286</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44287</v>
       </c>
@@ -457,91 +468,105 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>

</xml_diff>

<commit_message>
Index page was added for User Administration.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F38FA6-B409-454A-8A19-6162FC68321C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F118F5BF-6043-4003-A26A-B417C9D45C2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3315" yWindow="3315" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -382,7 +382,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,7 +487,7 @@
         <v>8</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Initial checkin for sales data service
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ErkoSMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\personal\Erko_Project\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F118F5BF-6043-4003-A26A-B417C9D45C2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371DF88F-EABE-4017-9DFA-10169A6475CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Developer1</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
   </si>
 </sst>
 </file>
@@ -382,16 +385,16 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="3" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -402,7 +405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>44272</v>
       </c>
@@ -413,7 +416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>44275</v>
       </c>
@@ -424,7 +427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>44283</v>
       </c>
@@ -435,7 +438,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44284</v>
       </c>
@@ -446,7 +449,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44286</v>
       </c>
@@ -457,7 +460,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44287</v>
       </c>
@@ -468,7 +471,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44289</v>
       </c>
@@ -479,7 +482,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44290</v>
       </c>
@@ -490,83 +493,88 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>44303</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
     </row>

</xml_diff>

<commit_message>
Sales list view is implemented (draft)
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\personal\Erko_Project\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371DF88F-EABE-4017-9DFA-10169A6475CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7890570B-646D-48B5-AD3F-4601C1667D37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29115" yWindow="1440" windowWidth="27000" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>Developer1</t>
   </si>
@@ -382,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,19 +503,39 @@
       <c r="C10" s="2"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11" s="2"/>
+      <c r="A11" s="1">
+        <v>44304</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
+      <c r="A12" s="1">
+        <v>44307</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
+      <c r="A13" s="1">
+        <v>44308</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
+      <c r="A14" s="1">
+        <v>44309</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -577,6 +597,10 @@
     <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Working hour is updated
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\personal\Erko_Project\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7A23B-CB82-4DBC-910D-19C2F151B8E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18743322-E5B6-4784-82F0-91C85919A5F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="360" windowWidth="23010" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>Developer1</t>
   </si>
@@ -34,33 +34,6 @@
   </si>
   <si>
     <t>Developer2</t>
-  </si>
-  <si>
-    <t>1.5</t>
-  </si>
-  <si>
-    <t>2.5</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>8</t>
   </si>
 </sst>
 </file>
@@ -102,10 +75,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -391,7 +367,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -440,71 +416,71 @@
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
+      <c r="C4" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>44284</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
+      <c r="B5" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>44286</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>4</v>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>44287</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>5</v>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>44289</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>7</v>
+      <c r="B8" s="3">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>44290</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>5</v>
+      <c r="B9" s="3">
+        <v>3</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>44303</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>9</v>
+      <c r="B10" s="3">
+        <v>4</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -512,8 +488,8 @@
       <c r="A11" s="1">
         <v>44304</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>7</v>
+      <c r="B11" s="3">
+        <v>1</v>
       </c>
       <c r="C11" s="2"/>
     </row>
@@ -521,8 +497,8 @@
       <c r="A12" s="1">
         <v>44307</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>4</v>
+      <c r="B12" s="3">
+        <v>2.5</v>
       </c>
       <c r="C12" s="2"/>
     </row>
@@ -530,8 +506,8 @@
       <c r="A13" s="1">
         <v>44308</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>9</v>
+      <c r="B13" s="3">
+        <v>4</v>
       </c>
       <c r="C13" s="2"/>
     </row>
@@ -539,8 +515,8 @@
       <c r="A14" s="1">
         <v>44309</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>9</v>
+      <c r="B14" s="3">
+        <v>4</v>
       </c>
       <c r="C14" s="2"/>
     </row>
@@ -548,8 +524,8 @@
       <c r="A15" s="1">
         <v>44332</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
+      <c r="B15" s="3">
+        <v>8</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -557,8 +533,8 @@
       <c r="A16" s="1">
         <v>44333</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
+      <c r="B16" s="3">
+        <v>8</v>
       </c>
       <c r="C16" s="2"/>
     </row>
@@ -566,13 +542,18 @@
       <c r="A17" s="1">
         <v>44334</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
+      <c r="B17" s="3">
+        <v>5</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
+      <c r="A18" s="1">
+        <v>44335</v>
+      </c>
+      <c r="B18" s="3">
+        <v>4</v>
+      </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Working hours are updated
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\personal\Erko_Project\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18743322-E5B6-4784-82F0-91C85919A5F0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0498FC-7D39-4947-AC58-3C15AEF3F4D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="360" windowWidth="23010" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -367,7 +367,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -552,7 +552,7 @@
         <v>44335</v>
       </c>
       <c r="B18" s="3">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2"/>
     </row>

</xml_diff>

<commit_message>
Purchase list screens are implemented. Purchace update screen is implemented (on-going) Workflow between order-purchase is implemented (on-going)
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\documents\personal\Erko_Project\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71ABF76-A9A6-41C0-8D6C-F6BB78B12E39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E3952E0-0FF6-45A0-A2CA-EBE4E0452F41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
     <t>Developer1</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>4</t>
+  </si>
+  <si>
+    <t>6</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -569,11 +572,21 @@
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
+      <c r="A20" s="1">
+        <v>44337</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B21" s="2"/>
+      <c r="A21" s="1">
+        <v>44338</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
SalesManStatistics view is implemented.
</commit_message>
<xml_diff>
--- a/WorkingHours.xlsx
+++ b/WorkingHours.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ErkoSMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A72C98-C8FA-4A23-8CF2-DFF7B7987F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717422F6-B9C3-4505-A682-833BFF9545D1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Developer1</t>
   </si>
@@ -48,9 +48,6 @@
   </si>
   <si>
     <t>İbrahim</t>
-  </si>
-  <si>
-    <t>2</t>
   </si>
 </sst>
 </file>
@@ -388,17 +385,17 @@
   <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -409,7 +406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>44272</v>
       </c>
@@ -420,7 +417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>44275</v>
       </c>
@@ -431,7 +428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>44283</v>
       </c>
@@ -442,7 +439,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>44284</v>
       </c>
@@ -453,7 +450,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>44286</v>
       </c>
@@ -464,7 +461,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>44287</v>
       </c>
@@ -475,7 +472,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>44289</v>
       </c>
@@ -486,7 +483,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>44290</v>
       </c>
@@ -497,7 +494,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>44294</v>
       </c>
@@ -506,7 +503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>44296</v>
       </c>
@@ -515,7 +512,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>44297</v>
       </c>
@@ -524,7 +521,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>44303</v>
       </c>
@@ -533,7 +530,7 @@
       </c>
       <c r="C13" s="5"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>44304</v>
       </c>
@@ -544,7 +541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>44305</v>
       </c>
@@ -553,7 +550,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>44307</v>
       </c>
@@ -562,7 +559,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>44308</v>
       </c>
@@ -571,7 +568,7 @@
       </c>
       <c r="C17" s="5"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>44309</v>
       </c>
@@ -584,10 +581,10 @@
       </c>
       <c r="J18" s="4">
         <f>SUM($C$2:$C$50)</f>
-        <v>51.5</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>55.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>44324</v>
       </c>
@@ -603,7 +600,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>44325</v>
       </c>
@@ -612,7 +609,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>44331</v>
       </c>
@@ -621,7 +618,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>44332</v>
       </c>
@@ -632,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>44333</v>
       </c>
@@ -643,7 +640,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>44334</v>
       </c>
@@ -652,7 +649,7 @@
       </c>
       <c r="C24" s="5"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>44335</v>
       </c>
@@ -663,7 +660,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>44336</v>
       </c>
@@ -674,7 +671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>44337</v>
       </c>
@@ -685,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>44338</v>
       </c>
@@ -696,7 +693,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>44339</v>
       </c>
@@ -707,7 +704,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>44340</v>
       </c>
@@ -716,44 +713,49 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>44341</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
+        <v>44345</v>
+      </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>

</xml_diff>